<commit_message>
first stab at fixing #4 (export fails if datamap different from col a in master)
</commit_message>
<xml_diff>
--- a/tests/resources/master.xlsx
+++ b/tests/resources/master.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="38">
   <si>
     <t xml:space="preserve">file name</t>
   </si>
@@ -28,30 +28,45 @@
     <t xml:space="preserve">Chutney Bridge.xlsm</t>
   </si>
   <si>
+    <t xml:space="preserve">Ramsbottom Knot Gorge Cleanout.xlsm</t>
+  </si>
+  <si>
     <t xml:space="preserve">Project/Programme Name</t>
   </si>
   <si>
     <t xml:space="preserve">Chutney Bridge Ltd</t>
   </si>
   <si>
+    <t xml:space="preserve">Ramsbottom Knot Gorge Cleanout Ltd</t>
+  </si>
+  <si>
     <t xml:space="preserve">Department </t>
   </si>
   <si>
     <t xml:space="preserve">Accounting Department</t>
   </si>
   <si>
+    <t xml:space="preserve">VA Department</t>
+  </si>
+  <si>
     <t xml:space="preserve">Delivery Body </t>
   </si>
   <si>
     <t xml:space="preserve">Satellite Corp</t>
   </si>
   <si>
+    <t xml:space="preserve">Hemptoast Market</t>
+  </si>
+  <si>
     <t xml:space="preserve">GMPP - IPA ID Number</t>
   </si>
   <si>
     <t xml:space="preserve">20A</t>
   </si>
   <si>
+    <t xml:space="preserve">22A</t>
+  </si>
+  <si>
     <t xml:space="preserve">Controls Project ID number</t>
   </si>
   <si>
@@ -85,6 +100,9 @@
     <t xml:space="preserve">Malcolm Tresseridge</t>
   </si>
   <si>
+    <t xml:space="preserve">Aiden P Tresseridge</t>
+  </si>
+  <si>
     <t xml:space="preserve">Senior Responsible Owner (SRO) - Email</t>
   </si>
   <si>
@@ -107,6 +125,9 @@
   </si>
   <si>
     <t xml:space="preserve">Bobbins</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Roadster</t>
   </si>
   <si>
     <t xml:space="preserve">Big Float</t>
@@ -123,11 +144,12 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="DD/MM/YY"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -146,9 +168,15 @@
     </font>
     <font>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -193,8 +221,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -202,7 +234,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -223,10 +255,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
+      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -243,154 +275,212 @@
       <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>7</v>
+        <v>10</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>9</v>
+        <v>13</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>1334</v>
       </c>
+      <c r="C6" s="0" t="n">
+        <v>13</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>12</v>
+        <v>17</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>14</v>
+        <v>19</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>16</v>
+        <v>21</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="B10" s="2" t="n">
+        <v>40909</v>
+      </c>
+      <c r="C10" s="2" t="n">
         <v>40909</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="B11" s="2" t="n">
+        <v>42798</v>
+      </c>
+      <c r="C11" s="2" t="n">
         <v>42798</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>20</v>
+        <v>25</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>22</v>
+        <v>27</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>20122</v>
       </c>
+      <c r="C14" s="0" t="n">
+        <v>2042</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="B15" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="B15" s="2" t="n">
+        <v>42653</v>
+      </c>
+      <c r="C15" s="2" t="n">
         <v>42653</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>26</v>
+        <v>32</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>28</v>
+        <v>34</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>20.303</v>
       </c>
+      <c r="C18" s="0" t="n">
+        <v>20.303</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="B19" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="B19" s="2" t="n">
+        <v>45323</v>
+      </c>
+      <c r="C19" s="2" t="n">
         <v>45323</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B13" r:id="rId1" display="mt@xclub.ck"/>
+    <hyperlink ref="C13" r:id="rId2" display="mt@xclub.ck"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>